<commit_message>
create new employee, assign leave &  verify it then delete that emp
</commit_message>
<xml_diff>
--- a/TrialOrangeHrm/src/main/java/com/hrm/qa/testdata/Test Data.xlsx
+++ b/TrialOrangeHrm/src/main/java/com/hrm/qa/testdata/Test Data.xlsx
@@ -4,8 +4,9 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="AssignLeaveDetails" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="NewUserDetails" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Emp Names" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="PerformanceTracker" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="NewUserDetails" sheetId="3" r:id="rId6"/>
+    <sheet state="visible" name="Emp Names" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr/>
@@ -13,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="115">
   <si>
     <t>TypeOfLeave</t>
   </si>
@@ -36,229 +37,280 @@
     <t>Maternity US</t>
   </si>
   <si>
+    <t>Nith Ya</t>
+  </si>
+  <si>
+    <t>2019-09-09</t>
+  </si>
+  <si>
+    <t>2019-09-10</t>
+  </si>
+  <si>
+    <t>Paternity US</t>
+  </si>
+  <si>
+    <t>Niki Tha</t>
+  </si>
+  <si>
+    <t>2019-10-07</t>
+  </si>
+  <si>
+    <t>2019-10-08</t>
+  </si>
+  <si>
+    <t>Vacation US</t>
+  </si>
+  <si>
+    <t>Narma Da</t>
+  </si>
+  <si>
+    <t>2019-11-25</t>
+  </si>
+  <si>
+    <t>2019-11-26</t>
+  </si>
+  <si>
+    <t>Nadhi Ya</t>
+  </si>
+  <si>
+    <t>2020-02-06</t>
+  </si>
+  <si>
+    <t>2020-02-07</t>
+  </si>
+  <si>
+    <t>2020-05-28</t>
+  </si>
+  <si>
+    <t>2020-05-29</t>
+  </si>
+  <si>
+    <t>2020-01-02</t>
+  </si>
+  <si>
+    <t>2020-01-03</t>
+  </si>
+  <si>
+    <t>2020-07-15</t>
+  </si>
+  <si>
+    <t>2020-07-17</t>
+  </si>
+  <si>
+    <t>2020-07-20</t>
+  </si>
+  <si>
+    <t>2020-07-22</t>
+  </si>
+  <si>
+    <t>2021-01-04</t>
+  </si>
+  <si>
+    <t>2021-01-05</t>
+  </si>
+  <si>
+    <t>TrackerName</t>
+  </si>
+  <si>
+    <t>EmpName</t>
+  </si>
+  <si>
+    <t>ReviewerName1</t>
+  </si>
+  <si>
+    <t>ReviewerName2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AM Shift Tracker </t>
+  </si>
+  <si>
+    <t>Linda Anderson</t>
+  </si>
+  <si>
+    <t>Test 1</t>
+  </si>
+  <si>
+    <t>PM Shift Tracker</t>
+  </si>
+  <si>
+    <t>John Smith</t>
+  </si>
+  <si>
+    <t>Robert Craig</t>
+  </si>
+  <si>
+    <t>ER Nurse Tracker</t>
+  </si>
+  <si>
+    <t>Hello World</t>
+  </si>
+  <si>
+    <t>Thomas Fleming</t>
+  </si>
+  <si>
+    <t>Peds Nurse Tracker</t>
+  </si>
+  <si>
+    <t>Hannah Flores</t>
+  </si>
+  <si>
+    <t>Fiona Grace</t>
+  </si>
+  <si>
+    <t>FirstName</t>
+  </si>
+  <si>
+    <t>LastName</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>FullName</t>
+  </si>
+  <si>
+    <t>Nith</t>
+  </si>
+  <si>
+    <t>Ya</t>
+  </si>
+  <si>
+    <t>C:/Users/browse/Pictures/WebPhotos/Tulips.jpg</t>
+  </si>
+  <si>
+    <t>nithya</t>
+  </si>
+  <si>
+    <t>Test@123!</t>
+  </si>
+  <si>
+    <t>Niki</t>
+  </si>
+  <si>
+    <t>Tha</t>
+  </si>
+  <si>
+    <t>C:/Users/browse/Pictures/WebPhotos/Poppy.jpg</t>
+  </si>
+  <si>
+    <t>nikitha</t>
+  </si>
+  <si>
+    <t>Test@123@</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Narma </t>
+  </si>
+  <si>
+    <t>Da</t>
+  </si>
+  <si>
+    <t>C:/Users/browse/Pictures/WebPhotos/Buttercups.jpg</t>
+  </si>
+  <si>
+    <t>narmada</t>
+  </si>
+  <si>
+    <t>Test@123#</t>
+  </si>
+  <si>
+    <t>Nadhi</t>
+  </si>
+  <si>
+    <t>C:/Users/browse/Pictures/WebPhotos/Daisies.jpg</t>
+  </si>
+  <si>
+    <t>nadhiya</t>
+  </si>
+  <si>
+    <t>Test@123$</t>
+  </si>
+  <si>
+    <t>Pree</t>
+  </si>
+  <si>
+    <t>preetha</t>
+  </si>
+  <si>
+    <t>Pree Tha</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pre </t>
+  </si>
+  <si>
+    <t>Ma</t>
+  </si>
+  <si>
+    <t>prema</t>
+  </si>
+  <si>
+    <t>Pre Ma</t>
+  </si>
+  <si>
+    <t>See</t>
+  </si>
+  <si>
+    <t>seetha</t>
+  </si>
+  <si>
+    <t>See Tha</t>
+  </si>
+  <si>
+    <t>Mee</t>
+  </si>
+  <si>
+    <t>Ta</t>
+  </si>
+  <si>
+    <t>meeta</t>
+  </si>
+  <si>
+    <t>Mee Ta</t>
+  </si>
+  <si>
+    <t>Shru</t>
+  </si>
+  <si>
+    <t>Thi</t>
+  </si>
+  <si>
+    <t>shruthi</t>
+  </si>
+  <si>
     <t>Shru Thi</t>
   </si>
   <si>
-    <t>2019-09-09</t>
-  </si>
-  <si>
-    <t>2019-09-10</t>
-  </si>
-  <si>
-    <t>Paternity US</t>
+    <t>Shri</t>
+  </si>
+  <si>
+    <t>shriya</t>
   </si>
   <si>
     <t>Shri Ya</t>
   </si>
   <si>
-    <t>2019-10-07</t>
-  </si>
-  <si>
-    <t>2019-10-08</t>
-  </si>
-  <si>
-    <t>Vacation US</t>
+    <t>Shwe</t>
+  </si>
+  <si>
+    <t>shwetha</t>
   </si>
   <si>
     <t>Shwe Tha</t>
   </si>
   <si>
-    <t>2019-11-25</t>
-  </si>
-  <si>
-    <t>2019-11-26</t>
+    <t>Smri</t>
+  </si>
+  <si>
+    <t>smrithi</t>
   </si>
   <si>
     <t>Smri Thi</t>
-  </si>
-  <si>
-    <t>2020-02-06</t>
-  </si>
-  <si>
-    <t>2020-02-07</t>
-  </si>
-  <si>
-    <t>2020-05-28</t>
-  </si>
-  <si>
-    <t>2020-05-29</t>
-  </si>
-  <si>
-    <t>2020-01-02</t>
-  </si>
-  <si>
-    <t>2020-01-03</t>
-  </si>
-  <si>
-    <t>2020-07-15</t>
-  </si>
-  <si>
-    <t>2020-07-17</t>
-  </si>
-  <si>
-    <t>2020-07-20</t>
-  </si>
-  <si>
-    <t>2020-07-22</t>
-  </si>
-  <si>
-    <t>2021-01-04</t>
-  </si>
-  <si>
-    <t>2021-01-05</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>Path</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>Shru</t>
-  </si>
-  <si>
-    <t>Thi</t>
-  </si>
-  <si>
-    <t>C:/Users/browse/Pictures/WebPhotos/Tulips.jpg</t>
-  </si>
-  <si>
-    <t>shruthi</t>
-  </si>
-  <si>
-    <t>Test@123!</t>
-  </si>
-  <si>
-    <t>Shri</t>
-  </si>
-  <si>
-    <t>Ya</t>
-  </si>
-  <si>
-    <t>C:/Users/browse/Pictures/WebPhotos/Poppy.jpg</t>
-  </si>
-  <si>
-    <t>shriya</t>
-  </si>
-  <si>
-    <t>Test@123@</t>
-  </si>
-  <si>
-    <t>Shwe</t>
-  </si>
-  <si>
-    <t>Tha</t>
-  </si>
-  <si>
-    <t>C:/Users/browse/Pictures/WebPhotos/Buttercups.jpg</t>
-  </si>
-  <si>
-    <t>shwetha</t>
-  </si>
-  <si>
-    <t>Test@123#</t>
-  </si>
-  <si>
-    <t>Smri</t>
-  </si>
-  <si>
-    <t>C:/Users/browse/Pictures/WebPhotos/Daisies.jpg</t>
-  </si>
-  <si>
-    <t>smrithi</t>
-  </si>
-  <si>
-    <t>Test@123$</t>
-  </si>
-  <si>
-    <t>Pree</t>
-  </si>
-  <si>
-    <t>preetha</t>
-  </si>
-  <si>
-    <t>Pree Tha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pre </t>
-  </si>
-  <si>
-    <t>Ma</t>
-  </si>
-  <si>
-    <t>prema</t>
-  </si>
-  <si>
-    <t>Pre Ma</t>
-  </si>
-  <si>
-    <t>See</t>
-  </si>
-  <si>
-    <t>seetha</t>
-  </si>
-  <si>
-    <t>See Tha</t>
-  </si>
-  <si>
-    <t>Mee</t>
-  </si>
-  <si>
-    <t>Ta</t>
-  </si>
-  <si>
-    <t>meeta</t>
-  </si>
-  <si>
-    <t>Mee Ta</t>
-  </si>
-  <si>
-    <t>Nith</t>
-  </si>
-  <si>
-    <t>nithya</t>
-  </si>
-  <si>
-    <t>Nith Ya</t>
-  </si>
-  <si>
-    <t>Niki</t>
-  </si>
-  <si>
-    <t>nikitha</t>
-  </si>
-  <si>
-    <t>Niki Tha</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Narma </t>
-  </si>
-  <si>
-    <t>Da</t>
-  </si>
-  <si>
-    <t>narmada</t>
-  </si>
-  <si>
-    <t>Narma Da</t>
-  </si>
-  <si>
-    <t>Nadhi</t>
-  </si>
-  <si>
-    <t>nadhiya</t>
-  </si>
-  <si>
-    <t>Nadhi Ya</t>
   </si>
   <si>
     <t>Ru</t>
@@ -347,14 +399,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFE06666"/>
-        <bgColor rgb="FFE06666"/>
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
-        <bgColor rgb="FFFFFFFF"/>
+        <fgColor rgb="FFE06666"/>
+        <bgColor rgb="FFE06666"/>
       </patternFill>
     </fill>
   </fills>
@@ -388,13 +440,13 @@
     <xf borderId="0" fillId="0" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+      <alignment horizontal="left" readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -412,6 +464,10 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
 </file>
 
@@ -868,113 +924,80 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="3" max="3" width="58.71"/>
+    <col customWidth="1" min="1" max="1" width="20.86"/>
+    <col customWidth="1" min="2" max="2" width="22.71"/>
+    <col customWidth="1" min="3" max="3" width="28.0"/>
+    <col customWidth="1" min="4" max="4" width="24.29"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="5" t="s">
         <v>33</v>
       </c>
       <c r="D1" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="9" t="s">
+    </row>
+    <row r="2">
+      <c r="A2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-    </row>
-    <row r="2">
-      <c r="A2" s="6" t="s">
+      <c r="B2" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="5" t="s">
+    </row>
+    <row r="3">
+      <c r="A3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="B3" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="D3" s="5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" s="6" t="s">
+    <row r="4">
+      <c r="A4" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B4" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D4" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="D3" s="6" t="s">
+    </row>
+    <row r="5">
+      <c r="A5" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="B5" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C4" s="11" t="s">
-        <v>48</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E4" s="5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -991,229 +1014,367 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="3" max="3" width="58.71"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
       <c r="A1" s="5" t="s">
-        <v>55</v>
+        <v>72</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>56</v>
+        <v>73</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>57</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="5" t="s">
-        <v>58</v>
+        <v>75</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>59</v>
+        <v>76</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>60</v>
+        <v>77</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>61</v>
+        <v>78</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="5" t="s">
-        <v>62</v>
+        <v>79</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>63</v>
+        <v>80</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>64</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="5" t="s">
-        <v>65</v>
+        <v>82</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>66</v>
+        <v>83</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>67</v>
+        <v>84</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>68</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="5" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="5" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>74</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="5" t="s">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>76</v>
+        <v>64</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>78</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="5" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>81</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="5" t="s">
-        <v>36</v>
+        <v>86</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>7</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="5" t="s">
-        <v>41</v>
+        <v>90</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>44</v>
+        <v>91</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>11</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="5" t="s">
-        <v>46</v>
+        <v>93</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>49</v>
+        <v>94</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="5" t="s">
-        <v>51</v>
+        <v>96</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>37</v>
+        <v>87</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>18</v>
+        <v>98</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="5" t="s">
-        <v>82</v>
+        <v>99</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="5" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>89</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="5" t="s">
-        <v>90</v>
+        <v>107</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>91</v>
+        <v>108</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>92</v>
+        <v>109</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="5" t="s">
-        <v>94</v>
+        <v>111</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>